<commit_message>
Week 2 Feedback incorporated as comments
</commit_message>
<xml_diff>
--- a/data/WEF_COVID_19_Risks_Outlook.xlsx
+++ b/data/WEF_COVID_19_Risks_Outlook.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernay/Desktop/DataViz/Repositories/Interactive-Data-Vis-Fall2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9314C3-FCC8-4048-8C2D-DE44C4FF3081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D9271-3423-894F-913E-AD94F6581D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="2100" windowWidth="35320" windowHeight="17480" xr2:uid="{A79B5F70-9CA4-F84F-A3BA-228B92A330B3}"/>
+    <workbookView xWindow="30600" yWindow="2100" windowWidth="35320" windowHeight="17480" activeTab="1" xr2:uid="{A79B5F70-9CA4-F84F-A3BA-228B92A330B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivoted" sheetId="5" r:id="rId1"/>
     <sheet name="Normalized" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Normalized!$A$1:$E$94</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -634,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF15680-E605-F14F-AD23-61DC923BEABA}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1325,10 +1328,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA5439D-12E3-D94B-95E8-67D10491FD49}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1360,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1392,7 +1396,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -1428,7 +1432,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1446,7 +1450,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1482,7 +1486,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1500,7 +1504,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1518,7 +1522,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -1572,7 +1576,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -1590,7 +1594,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1662,7 +1666,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1698,7 +1702,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1720,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1734,7 +1738,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1752,7 +1756,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1788,7 +1792,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -1806,7 +1810,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1914,7 +1918,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
@@ -1950,7 +1954,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
@@ -1986,7 +1990,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -2004,7 +2008,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -2058,7 +2062,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -2076,7 +2080,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>36</v>
       </c>
@@ -2094,7 +2098,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>36</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
@@ -2148,7 +2152,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>36</v>
       </c>
@@ -2166,7 +2170,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>36</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>36</v>
       </c>
@@ -2202,7 +2206,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>36</v>
       </c>
@@ -2220,7 +2224,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>36</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>36</v>
       </c>
@@ -2256,7 +2260,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>36</v>
       </c>
@@ -2274,7 +2278,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>36</v>
       </c>
@@ -2292,7 +2296,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>36</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>36</v>
       </c>
@@ -2382,7 +2386,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>36</v>
       </c>
@@ -2400,7 +2404,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>36</v>
       </c>
@@ -2418,7 +2422,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>36</v>
       </c>
@@ -2436,7 +2440,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>36</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>36</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>37</v>
       </c>
@@ -2508,7 +2512,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>37</v>
       </c>
@@ -2526,7 +2530,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>37</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -2562,7 +2566,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>37</v>
       </c>
@@ -2580,7 +2584,7 @@
         <v>High</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>37</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>37</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>37</v>
       </c>
@@ -2634,7 +2638,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>37</v>
       </c>
@@ -2652,7 +2656,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>37</v>
       </c>
@@ -2670,7 +2674,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>37</v>
       </c>
@@ -2688,7 +2692,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -2706,7 +2710,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -2724,7 +2728,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2742,7 +2746,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -2760,7 +2764,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -2796,7 +2800,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>37</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2850,7 +2854,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>37</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>37</v>
       </c>
@@ -2904,7 +2908,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>37</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2940,7 +2944,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>37</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>37</v>
       </c>
@@ -2994,7 +2998,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>37</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>37</v>
       </c>
@@ -3031,6 +3035,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E94" xr:uid="{6F699A09-FC62-F044-B6DD-38888CEEE27D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Environmental"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>